<commit_message>
reorganization plot glacial-interglacial paleosol-CO2 record
</commit_message>
<xml_diff>
--- a/data/Dataset S1.xlsx
+++ b/data/Dataset S1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiawei/Documents/Work/2019- glacial CO2/Glacial_CO2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4C3758-48DD-DF4E-BBC0-C28F5AE0A8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7430F8C-FB08-7F4B-A6B1-CCB88000878D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="-20160" windowWidth="21000" windowHeight="18880" activeTab="1" xr2:uid="{F264F01B-AE22-4945-AD16-2719434C6BE8}"/>
+    <workbookView xWindow="11260" yWindow="640" windowWidth="30240" windowHeight="19640" activeTab="1" xr2:uid="{F264F01B-AE22-4945-AD16-2719434C6BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="800ky" sheetId="1" r:id="rId1"/>
@@ -3234,9 +3234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0910CBD0-BDC1-514A-8AB0-A05DF07425DA}">
   <dimension ref="A1:W149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U119" sqref="U119"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R130" sqref="R130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3363,10 +3363,10 @@
         <v>0.11774306683324098</v>
       </c>
       <c r="O2" s="20">
-        <v>277.098059895147</v>
+        <v>275.05990892102301</v>
       </c>
       <c r="P2" s="20">
-        <v>163.64866070728701</v>
+        <v>166.523728560444</v>
       </c>
       <c r="Q2" s="20">
         <v>285.74249746790798</v>
@@ -3430,10 +3430,10 @@
         <v>7.2110459750780009E-2</v>
       </c>
       <c r="O3" s="20">
-        <v>323.06318300313802</v>
+        <v>325.81563693649099</v>
       </c>
       <c r="P3" s="20">
-        <v>212.62966675698701</v>
+        <v>212.12865302913499</v>
       </c>
       <c r="Q3" s="20">
         <v>254.111915585606</v>
@@ -3497,10 +3497,10 @@
         <v>7.7552290842182958E-2</v>
       </c>
       <c r="O4" s="20">
-        <v>343.547262795623</v>
+        <v>339.990327233926</v>
       </c>
       <c r="P4" s="20">
-        <v>228.22063531639299</v>
+        <v>223.86336215905001</v>
       </c>
       <c r="Q4" s="20">
         <v>273.044968232158</v>
@@ -3564,10 +3564,10 @@
         <v>8.2219838398265965E-2</v>
       </c>
       <c r="O5" s="20">
-        <v>294.390321744125</v>
+        <v>293.99582117641501</v>
       </c>
       <c r="P5" s="20">
-        <v>182.08028559034901</v>
+        <v>181.966673621826</v>
       </c>
       <c r="Q5" s="20">
         <v>257.96354774874601</v>
@@ -3631,10 +3631,10 @@
         <v>8.275869751950593E-2</v>
       </c>
       <c r="O6" s="20">
-        <v>359.61749823993</v>
+        <v>357.498194007503</v>
       </c>
       <c r="P6" s="20">
-        <v>235.00859962950099</v>
+        <v>241.259013827225</v>
       </c>
       <c r="Q6" s="20">
         <v>266.82227324807701</v>
@@ -3698,10 +3698,10 @@
         <v>8.6104975660626026E-2</v>
       </c>
       <c r="O7" s="20">
-        <v>357.95670688528702</v>
+        <v>357.74276472431399</v>
       </c>
       <c r="P7" s="20">
-        <v>236.78030689372099</v>
+        <v>236.38788892898299</v>
       </c>
       <c r="Q7" s="20">
         <v>277.53761243685602</v>
@@ -3765,10 +3765,10 @@
         <v>8.7052890623066981E-2</v>
       </c>
       <c r="O8" s="20">
-        <v>287.96589686199502</v>
+        <v>287.215466229605</v>
       </c>
       <c r="P8" s="20">
-        <v>173.902060348731</v>
+        <v>176.117509144216</v>
       </c>
       <c r="Q8" s="20">
         <v>224.73831148055501</v>
@@ -3832,10 +3832,10 @@
         <v>7.5501759071539998E-2</v>
       </c>
       <c r="O9" s="20">
-        <v>321.93590400280101</v>
+        <v>322.150738479425</v>
       </c>
       <c r="P9" s="20">
-        <v>205.578385066214</v>
+        <v>205.51369977973201</v>
       </c>
       <c r="Q9" s="20">
         <v>235.91536052685299</v>
@@ -3899,10 +3899,10 @@
         <v>7.4618029737118952E-2</v>
       </c>
       <c r="O10" s="20">
-        <v>298.88429909265602</v>
+        <v>299.629608293442</v>
       </c>
       <c r="P10" s="20">
-        <v>182.68167872756001</v>
+        <v>185.40757902392301</v>
       </c>
       <c r="Q10" s="20">
         <v>226.556047922201</v>
@@ -3966,10 +3966,10 @@
         <v>7.8838604618668984E-2</v>
       </c>
       <c r="O11" s="20">
-        <v>362.97473631237301</v>
+        <v>363.49977110362698</v>
       </c>
       <c r="P11" s="20">
-        <v>242.014078210468</v>
+        <v>245.52908777209399</v>
       </c>
       <c r="Q11" s="20">
         <v>275.422213316382</v>
@@ -4033,10 +4033,10 @@
         <v>8.7129658259115006E-2</v>
       </c>
       <c r="O12" s="20">
-        <v>323.249277178049</v>
+        <v>321.38053533315002</v>
       </c>
       <c r="P12" s="20">
-        <v>209.160678439203</v>
+        <v>206.547739734017</v>
       </c>
       <c r="Q12" s="20">
         <v>269.44364703486599</v>
@@ -4100,10 +4100,10 @@
         <v>7.955409812932801E-2</v>
       </c>
       <c r="O13" s="20">
-        <v>388.60011311492002</v>
+        <v>382.51989351144698</v>
       </c>
       <c r="P13" s="20">
-        <v>265.30754287436901</v>
+        <v>261.75983747149701</v>
       </c>
       <c r="Q13" s="20">
         <v>270.886424382548</v>
@@ -4167,10 +4167,10 @@
         <v>6.3518858556129043E-2</v>
       </c>
       <c r="O14" s="20">
-        <v>358.62470991794999</v>
+        <v>355.47543979311502</v>
       </c>
       <c r="P14" s="20">
-        <v>232.98584373611101</v>
+        <v>242.26856124225401</v>
       </c>
       <c r="Q14" s="20">
         <v>246.42809520637101</v>
@@ -4234,10 +4234,10 @@
         <v>7.494963798696197E-2</v>
       </c>
       <c r="O15" s="20">
-        <v>340.30665618287497</v>
+        <v>346.28910004608298</v>
       </c>
       <c r="P15" s="20">
-        <v>233.041553469375</v>
+        <v>226.19160029471499</v>
       </c>
       <c r="Q15" s="20">
         <v>279.54670393407798</v>
@@ -4301,10 +4301,10 @@
         <v>6.7591304232513028E-2</v>
       </c>
       <c r="O16" s="20">
-        <v>305.71395008681401</v>
+        <v>306.81579952877399</v>
       </c>
       <c r="P16" s="20">
-        <v>191.89785048746299</v>
+        <v>190.246435038588</v>
       </c>
       <c r="Q16" s="20">
         <v>202.35950858367201</v>
@@ -4368,10 +4368,10 @@
         <v>7.5299378924631011E-2</v>
       </c>
       <c r="O17" s="20">
-        <v>300.50158534382598</v>
+        <v>301.551011367456</v>
       </c>
       <c r="P17" s="20">
-        <v>186.716977005247</v>
+        <v>190.008478346348</v>
       </c>
       <c r="Q17" s="20">
         <v>239.79874676652599</v>
@@ -4435,10 +4435,10 @@
         <v>6.9790001252274969E-2</v>
       </c>
       <c r="O18" s="20">
-        <v>365.64453088107001</v>
+        <v>360.89349533282802</v>
       </c>
       <c r="P18" s="20">
-        <v>245.530355133603</v>
+        <v>243.355675720042</v>
       </c>
       <c r="Q18" s="20">
         <v>268.94134917631698</v>
@@ -4502,10 +4502,10 @@
         <v>0.11040031056381205</v>
       </c>
       <c r="O19" s="20">
-        <v>305.18124033696898</v>
+        <v>304.65805920557602</v>
       </c>
       <c r="P19" s="20">
-        <v>190.61862794819999</v>
+        <v>188.73601720493801</v>
       </c>
       <c r="Q19" s="20">
         <v>288.22822347184899</v>
@@ -4569,10 +4569,10 @@
         <v>8.2403052213596006E-2</v>
       </c>
       <c r="O20" s="20">
-        <v>327.85301419599898</v>
+        <v>327.45187615769999</v>
       </c>
       <c r="P20" s="20">
-        <v>213.44428860402701</v>
+        <v>210.179153987018</v>
       </c>
       <c r="Q20" s="20">
         <v>283.88629430072501</v>
@@ -4636,10 +4636,10 @@
         <v>8.1637053179921981E-2</v>
       </c>
       <c r="O21" s="20">
-        <v>355.012881508183</v>
+        <v>352.069132966719</v>
       </c>
       <c r="P21" s="20">
-        <v>238.73441539143801</v>
+        <v>234.17804471120201</v>
       </c>
       <c r="Q21" s="20">
         <v>300.13363940392202</v>
@@ -4703,10 +4703,10 @@
         <v>8.4913109881111004E-2</v>
       </c>
       <c r="O22" s="20">
-        <v>333.73612742995198</v>
+        <v>333.72940592007598</v>
       </c>
       <c r="P22" s="20">
-        <v>215.720054040121</v>
+        <v>215.047972899097</v>
       </c>
       <c r="Q22" s="20">
         <v>290.99315701149101</v>
@@ -4770,10 +4770,10 @@
         <v>6.8141184372843E-2</v>
       </c>
       <c r="O23" s="20">
-        <v>362.96539582858099</v>
+        <v>353.89820295305702</v>
       </c>
       <c r="P23" s="20">
-        <v>236.164111577017</v>
+        <v>236.38228787383201</v>
       </c>
       <c r="Q23" s="20">
         <v>232.404493540282</v>
@@ -4837,10 +4837,10 @@
         <v>7.5702762690264991E-2</v>
       </c>
       <c r="O24" s="20">
-        <v>390.85648214902</v>
+        <v>391.10424819921701</v>
       </c>
       <c r="P24" s="20">
-        <v>266.61768009479999</v>
+        <v>269.48989287806302</v>
       </c>
       <c r="Q24" s="20">
         <v>284.94161792192801</v>
@@ -4904,10 +4904,10 @@
         <v>6.6009546864687962E-2</v>
       </c>
       <c r="O25" s="20">
-        <v>345.157873564569</v>
+        <v>352.39333883828101</v>
       </c>
       <c r="P25" s="20">
-        <v>233.28481969972199</v>
+        <v>230.52985261430501</v>
       </c>
       <c r="Q25" s="20">
         <v>263.85056536792803</v>
@@ -4971,10 +4971,10 @@
         <v>7.1870612011475044E-2</v>
       </c>
       <c r="O26" s="20">
-        <v>371.64175143434102</v>
+        <v>370.721235034816</v>
       </c>
       <c r="P26" s="20">
-        <v>253.10206206139</v>
+        <v>249.72012505790599</v>
       </c>
       <c r="Q26" s="20">
         <v>274.31904179402602</v>
@@ -5038,10 +5038,10 @@
         <v>7.4181746142529037E-2</v>
       </c>
       <c r="O27" s="20">
-        <v>345.82580363280402</v>
+        <v>341.120510421787</v>
       </c>
       <c r="P27" s="20">
-        <v>220.26006477316099</v>
+        <v>220.93533053870701</v>
       </c>
       <c r="Q27" s="20">
         <v>291.368249629834</v>
@@ -5105,10 +5105,10 @@
         <v>7.6426787090498993E-2</v>
       </c>
       <c r="O28" s="20">
-        <v>332.02477792684101</v>
+        <v>327.80829464249803</v>
       </c>
       <c r="P28" s="20">
-        <v>211.464078615939</v>
+        <v>209.13796923953001</v>
       </c>
       <c r="Q28" s="20">
         <v>241.338373458446</v>
@@ -5172,10 +5172,10 @@
         <v>9.3251237190713043E-2</v>
       </c>
       <c r="O29" s="20">
-        <v>369.65188401175197</v>
+        <v>375.09245394928303</v>
       </c>
       <c r="P29" s="20">
-        <v>250.696245597955</v>
+        <v>249.39165189553901</v>
       </c>
       <c r="Q29" s="20">
         <v>285.747528614614</v>
@@ -5239,10 +5239,10 @@
         <v>9.5902953402935975E-2</v>
       </c>
       <c r="O30" s="20">
-        <v>331.083435096779</v>
+        <v>324.93825963798002</v>
       </c>
       <c r="P30" s="20">
-        <v>209.29360287336499</v>
+        <v>211.47708329814699</v>
       </c>
       <c r="Q30" s="20">
         <v>282.44175835299097</v>
@@ -5306,10 +5306,10 @@
         <v>8.2544145506610045E-2</v>
       </c>
       <c r="O31" s="20">
-        <v>381.326480825403</v>
+        <v>374.64466078528102</v>
       </c>
       <c r="P31" s="20">
-        <v>263.71029651651202</v>
+        <v>258.97010099462801</v>
       </c>
       <c r="Q31" s="20">
         <v>289.56687490125802</v>
@@ -5373,10 +5373,10 @@
         <v>8.9009107644232976E-2</v>
       </c>
       <c r="O32" s="20">
-        <v>363.25038353475998</v>
+        <v>360.80311147788598</v>
       </c>
       <c r="P32" s="20">
-        <v>237.677722609733</v>
+        <v>235.40995306655</v>
       </c>
       <c r="Q32" s="20">
         <v>301.51702943857202</v>
@@ -5440,10 +5440,10 @@
         <v>7.4022408247875982E-2</v>
       </c>
       <c r="O33" s="20">
-        <v>325.46490890830898</v>
+        <v>328.443645847261</v>
       </c>
       <c r="P33" s="20">
-        <v>208.79718250738401</v>
+        <v>208.76553576671699</v>
       </c>
       <c r="Q33" s="20">
         <v>286.97227343992398</v>
@@ -5507,10 +5507,10 @@
         <v>7.4485018480038967E-2</v>
       </c>
       <c r="O34" s="20">
-        <v>351.970369065554</v>
+        <v>355.93531181943399</v>
       </c>
       <c r="P34" s="20">
-        <v>237.452613327352</v>
+        <v>232.84504573319199</v>
       </c>
       <c r="Q34" s="20">
         <v>289.41368567135697</v>
@@ -5574,10 +5574,10 @@
         <v>8.7232352287009984E-2</v>
       </c>
       <c r="O35" s="20">
-        <v>345.38825788466897</v>
+        <v>345.76146147804297</v>
       </c>
       <c r="P35" s="20">
-        <v>228.24390204568499</v>
+        <v>229.97524803207801</v>
       </c>
       <c r="Q35" s="20">
         <v>286.35488969491001</v>
@@ -5641,10 +5641,10 @@
         <v>7.8969784829205913E-2</v>
       </c>
       <c r="O36" s="20">
-        <v>363.275785923417</v>
+        <v>360.124593796093</v>
       </c>
       <c r="P36" s="20">
-        <v>240.680677268761</v>
+        <v>237.97634436231601</v>
       </c>
       <c r="Q36" s="20">
         <v>275.97922037085698</v>
@@ -5708,10 +5708,10 @@
         <v>8.3922007514109054E-2</v>
       </c>
       <c r="O37" s="20">
-        <v>311.03792118654002</v>
+        <v>309.80851572037801</v>
       </c>
       <c r="P37" s="20">
-        <v>194.42646207617199</v>
+        <v>196.761751109637</v>
       </c>
       <c r="Q37" s="20">
         <v>257.06489531037101</v>
@@ -5775,10 +5775,10 @@
         <v>6.7179236256302954E-2</v>
       </c>
       <c r="O38" s="20">
-        <v>331.23919078294301</v>
+        <v>328.66081187706197</v>
       </c>
       <c r="P38" s="20">
-        <v>216.76395244944001</v>
+        <v>212.78024415860801</v>
       </c>
       <c r="Q38" s="20">
         <v>263.539041171799</v>
@@ -5842,10 +5842,10 @@
         <v>6.6758983342224076E-2</v>
       </c>
       <c r="O39" s="20">
-        <v>332.07845968915399</v>
+        <v>329.36065705008798</v>
       </c>
       <c r="P39" s="20">
-        <v>216.21127625752899</v>
+        <v>216.78109120714399</v>
       </c>
       <c r="Q39" s="20">
         <v>267.41777170965702</v>
@@ -5909,10 +5909,10 @@
         <v>7.2581718884781043E-2</v>
       </c>
       <c r="O40" s="20">
-        <v>299.97183179029901</v>
+        <v>300.914648628534</v>
       </c>
       <c r="P40" s="20">
-        <v>185.331585037509</v>
+        <v>183.32643826908199</v>
       </c>
       <c r="Q40" s="20">
         <v>274.44076053746602</v>
@@ -5976,10 +5976,10 @@
         <v>7.0831360153829959E-2</v>
       </c>
       <c r="O41" s="20">
-        <v>278.57418279442101</v>
+        <v>277.09266605820801</v>
       </c>
       <c r="P41" s="20">
-        <v>167.55955226123299</v>
+        <v>168.707081717752</v>
       </c>
       <c r="Q41" s="20">
         <v>250.684309846986</v>
@@ -6043,10 +6043,10 @@
         <v>7.4821679672221975E-2</v>
       </c>
       <c r="O42" s="20">
-        <v>277.66867939413402</v>
+        <v>276.37159083058299</v>
       </c>
       <c r="P42" s="20">
-        <v>166.35474039722001</v>
+        <v>166.100298704284</v>
       </c>
       <c r="Q42" s="20">
         <v>256.48858690446701</v>
@@ -6110,10 +6110,10 @@
         <v>7.7143465245062992E-2</v>
       </c>
       <c r="O43" s="20">
-        <v>299.37887015001502</v>
+        <v>293.84381746517403</v>
       </c>
       <c r="P43" s="20">
-        <v>186.24359883837499</v>
+        <v>185.90381716844999</v>
       </c>
       <c r="Q43" s="20">
         <v>284.09181635291799</v>
@@ -6177,10 +6177,10 @@
         <v>8.0717798041996081E-2</v>
       </c>
       <c r="O44" s="20">
-        <v>301.48935611833701</v>
+        <v>301.76971217555598</v>
       </c>
       <c r="P44" s="20">
-        <v>189.01282999298701</v>
+        <v>188.76995178429999</v>
       </c>
       <c r="Q44" s="20">
         <v>263.974904521143</v>
@@ -6244,10 +6244,10 @@
         <v>8.375588587552496E-2</v>
       </c>
       <c r="O45" s="20">
-        <v>302.42065855016898</v>
+        <v>306.30040885535499</v>
       </c>
       <c r="P45" s="20">
-        <v>187.874409158822</v>
+        <v>189.79229125605201</v>
       </c>
       <c r="Q45" s="20">
         <v>288.96449340846198</v>
@@ -6311,10 +6311,10 @@
         <v>8.3838896830189968E-2</v>
       </c>
       <c r="O46" s="20">
-        <v>310.659937344931</v>
+        <v>307.33672794812998</v>
       </c>
       <c r="P46" s="20">
-        <v>193.18434876178901</v>
+        <v>187.168533106864</v>
       </c>
       <c r="Q46" s="20">
         <v>308.14782480788102</v>
@@ -6378,10 +6378,10 @@
         <v>7.3377661046107989E-2</v>
       </c>
       <c r="O47" s="20">
-        <v>295.08688307838702</v>
+        <v>296.12691187565798</v>
       </c>
       <c r="P47" s="20">
-        <v>180.85050359720199</v>
+        <v>186.27353149578801</v>
       </c>
       <c r="Q47" s="20">
         <v>278.570412621711</v>
@@ -6445,10 +6445,10 @@
         <v>7.9228865817297933E-2</v>
       </c>
       <c r="O48" s="20">
-        <v>301.22949031644703</v>
+        <v>300.95510185771798</v>
       </c>
       <c r="P48" s="20">
-        <v>184.332957404008</v>
+        <v>183.264275486526</v>
       </c>
       <c r="Q48" s="20">
         <v>291.61177588352501</v>
@@ -6512,10 +6512,10 @@
         <v>7.1346331949414976E-2</v>
       </c>
       <c r="O49" s="20">
-        <v>304.11057825585601</v>
+        <v>306.27558209614898</v>
       </c>
       <c r="P49" s="20">
-        <v>190.63463765779301</v>
+        <v>191.75075979155099</v>
       </c>
       <c r="Q49" s="20">
         <v>234.04054135673101</v>
@@ -6579,10 +6579,10 @@
         <v>7.3538118434501976E-2</v>
       </c>
       <c r="O50" s="20">
-        <v>331.38828516283399</v>
+        <v>333.45173177853002</v>
       </c>
       <c r="P50" s="20">
-        <v>212.70331798585201</v>
+        <v>213.71409031483799</v>
       </c>
       <c r="Q50" s="20">
         <v>289.46733947584698</v>
@@ -6646,10 +6646,10 @@
         <v>6.8000795419940085E-2</v>
       </c>
       <c r="O51" s="20">
-        <v>310.43320412276</v>
+        <v>304.416012579187</v>
       </c>
       <c r="P51" s="20">
-        <v>193.51541653580901</v>
+        <v>194.625870192696</v>
       </c>
       <c r="Q51" s="20">
         <v>262.42944086789402</v>
@@ -6713,10 +6713,10 @@
         <v>6.664180062017E-2</v>
       </c>
       <c r="O52" s="20">
-        <v>311.95307817815899</v>
+        <v>309.28452119160397</v>
       </c>
       <c r="P52" s="20">
-        <v>195.05876673181501</v>
+        <v>199.802524127737</v>
       </c>
       <c r="Q52" s="20">
         <v>226.91014854348799</v>
@@ -6780,10 +6780,10 @@
         <v>7.7010971835215103E-2</v>
       </c>
       <c r="O53" s="20">
-        <v>333.91373415036998</v>
+        <v>332.49169192137998</v>
       </c>
       <c r="P53" s="20">
-        <v>219.39827560087099</v>
+        <v>218.35788905044501</v>
       </c>
       <c r="Q53" s="20">
         <v>329.71536944375799</v>
@@ -6847,10 +6847,10 @@
         <v>7.052372416546604E-2</v>
       </c>
       <c r="O54" s="20">
-        <v>362.62758902538002</v>
+        <v>359.87637493102</v>
       </c>
       <c r="P54" s="20">
-        <v>243.53839515152501</v>
+        <v>242.387563502977</v>
       </c>
       <c r="Q54" s="20">
         <v>263.48024953387898</v>
@@ -6914,10 +6914,10 @@
         <v>7.1537775912013934E-2</v>
       </c>
       <c r="O55" s="20">
-        <v>341.02796704484501</v>
+        <v>338.71538918904702</v>
       </c>
       <c r="P55" s="20">
-        <v>225.07585619999</v>
+        <v>226.97022435612701</v>
       </c>
       <c r="Q55" s="20">
         <v>299.61708145275401</v>
@@ -6981,10 +6981,10 @@
         <v>8.0758809404192888E-2</v>
       </c>
       <c r="O56" s="20">
-        <v>268.21497521382202</v>
+        <v>262.63890665392</v>
       </c>
       <c r="P56" s="20">
-        <v>158.19083259496901</v>
+        <v>157.048237202123</v>
       </c>
       <c r="Q56" s="20">
         <v>270.427190850486</v>
@@ -7048,10 +7048,10 @@
         <v>7.8285924278923003E-2</v>
       </c>
       <c r="O57" s="20">
-        <v>284.68718645471603</v>
+        <v>282.35058769012602</v>
       </c>
       <c r="P57" s="20">
-        <v>174.77829662387501</v>
+        <v>175.46105405070199</v>
       </c>
       <c r="Q57" s="20">
         <v>270.27000846420998</v>
@@ -7115,10 +7115,10 @@
         <v>8.2120473987596032E-2</v>
       </c>
       <c r="O58" s="20">
-        <v>335.49205197421298</v>
+        <v>330.42120852423199</v>
       </c>
       <c r="P58" s="20">
-        <v>218.24805131132001</v>
+        <v>215.709649020494</v>
       </c>
       <c r="Q58" s="20">
         <v>241.885857568414</v>
@@ -7182,10 +7182,10 @@
         <v>9.0879511569911031E-2</v>
       </c>
       <c r="O59" s="20">
-        <v>333.043261557628</v>
+        <v>331.86269099926199</v>
       </c>
       <c r="P59" s="20">
-        <v>215.36241354572601</v>
+        <v>210.20260150172399</v>
       </c>
       <c r="Q59" s="20">
         <v>298.69813236105199</v>
@@ -7249,10 +7249,10 @@
         <v>9.1082029055707059E-2</v>
       </c>
       <c r="O60" s="20">
-        <v>299.74064489662601</v>
+        <v>296.31545255588202</v>
       </c>
       <c r="P60" s="20">
-        <v>184.809808445611</v>
+        <v>183.874054844303</v>
       </c>
       <c r="Q60" s="20">
         <v>291.55342949592699</v>
@@ -7316,10 +7316,10 @@
         <v>8.7863612522901979E-2</v>
       </c>
       <c r="O61" s="20">
-        <v>299.48291452050597</v>
+        <v>299.68192030569901</v>
       </c>
       <c r="P61" s="20">
-        <v>188.76118162370801</v>
+        <v>186.99591749637199</v>
       </c>
       <c r="Q61" s="20">
         <v>322.83417412062801</v>
@@ -7383,10 +7383,10 @@
         <v>7.8538517589631041E-2</v>
       </c>
       <c r="O62" s="20">
-        <v>333.254735102057</v>
+        <v>330.422040429584</v>
       </c>
       <c r="P62" s="20">
-        <v>218.19665115968601</v>
+        <v>214.82355073194699</v>
       </c>
       <c r="Q62" s="20">
         <v>313.04241651371302</v>
@@ -7450,10 +7450,10 @@
         <v>7.7373441536981002E-2</v>
       </c>
       <c r="O63" s="20">
-        <v>330.01322667897102</v>
+        <v>330.398841904964</v>
       </c>
       <c r="P63" s="20">
-        <v>215.934008096946</v>
+        <v>210.64870856802901</v>
       </c>
       <c r="Q63" s="20">
         <v>320.83307675805099</v>
@@ -7517,10 +7517,10 @@
         <v>7.1245843589723079E-2</v>
       </c>
       <c r="O64" s="20">
-        <v>327.80374715432299</v>
+        <v>325.90217378016399</v>
       </c>
       <c r="P64" s="20">
-        <v>205.86043101555501</v>
+        <v>209.57718425395501</v>
       </c>
       <c r="Q64" s="20">
         <v>255.308256976031</v>
@@ -7584,10 +7584,10 @@
         <v>7.5642992235238071E-2</v>
       </c>
       <c r="O65" s="20">
-        <v>363.64355494951599</v>
+        <v>359.45177444455601</v>
       </c>
       <c r="P65" s="20">
-        <v>244.00743010267999</v>
+        <v>244.90205406191501</v>
       </c>
       <c r="Q65" s="20">
         <v>338.06961645411099</v>
@@ -7651,10 +7651,10 @@
         <v>8.1754931865991032E-2</v>
       </c>
       <c r="O66" s="20">
-        <v>327.64787017138201</v>
+        <v>327.56955941678001</v>
       </c>
       <c r="P66" s="20">
-        <v>211.17627406146499</v>
+        <v>211.19978502770499</v>
       </c>
       <c r="Q66" s="20">
         <v>316.43494152369402</v>
@@ -7718,10 +7718,10 @@
         <v>8.1421022819714084E-2</v>
       </c>
       <c r="O67" s="20">
-        <v>330.21863933105197</v>
+        <v>331.21792502729301</v>
       </c>
       <c r="P67" s="20">
-        <v>215.24540908291399</v>
+        <v>214.75829977227099</v>
       </c>
       <c r="Q67" s="20">
         <v>341.93787305811401</v>
@@ -7785,10 +7785,10 @@
         <v>7.6922726685330067E-2</v>
       </c>
       <c r="O68" s="20">
-        <v>335.51166615669399</v>
+        <v>335.81040111117699</v>
       </c>
       <c r="P68" s="20">
-        <v>216.68265776049799</v>
+        <v>215.730893511327</v>
       </c>
       <c r="Q68" s="20">
         <v>296.91039781800902</v>
@@ -7852,10 +7852,10 @@
         <v>8.4082690102728952E-2</v>
       </c>
       <c r="O69" s="20">
-        <v>329.14269290843998</v>
+        <v>333.71742555690298</v>
       </c>
       <c r="P69" s="20">
-        <v>209.59511183684799</v>
+        <v>211.859827986048</v>
       </c>
       <c r="Q69" s="20">
         <v>334.11714743789599</v>
@@ -7919,10 +7919,10 @@
         <v>8.9923806581170052E-2</v>
       </c>
       <c r="O70" s="20">
-        <v>338.32413673187102</v>
+        <v>337.592376592731</v>
       </c>
       <c r="P70" s="20">
-        <v>224.72229340759401</v>
+        <v>222.245087584982</v>
       </c>
       <c r="Q70" s="20">
         <v>407.26177743657303</v>
@@ -7986,10 +7986,10 @@
         <v>9.3302347319379919E-2</v>
       </c>
       <c r="O71" s="20">
-        <v>324.58070352782198</v>
+        <v>327.72041393364299</v>
       </c>
       <c r="P71" s="20">
-        <v>206.65698068394099</v>
+        <v>209.15437663579399</v>
       </c>
       <c r="Q71" s="20">
         <v>405.24208056261</v>
@@ -8053,10 +8053,10 @@
         <v>8.5204731056319982E-2</v>
       </c>
       <c r="O72" s="20">
-        <v>343.64138318883198</v>
+        <v>346.541360242081</v>
       </c>
       <c r="P72" s="20">
-        <v>229.11312282921901</v>
+        <v>224.552679516929</v>
       </c>
       <c r="Q72" s="20">
         <v>380.343097896156</v>
@@ -8120,10 +8120,10 @@
         <v>9.3846989242611034E-2</v>
       </c>
       <c r="O73" s="20">
-        <v>318.759468050007</v>
+        <v>320.45779969911098</v>
       </c>
       <c r="P73" s="20">
-        <v>203.156651261261</v>
+        <v>202.46763575111399</v>
       </c>
       <c r="Q73" s="20">
         <v>338.14930671382001</v>
@@ -8187,10 +8187,10 @@
         <v>7.6912516792689956E-2</v>
       </c>
       <c r="O74" s="20">
-        <v>294.93915852174598</v>
+        <v>296.455263632271</v>
       </c>
       <c r="P74" s="20">
-        <v>181.82008461592901</v>
+        <v>181.23156627420801</v>
       </c>
       <c r="Q74" s="20">
         <v>282.42049043828598</v>
@@ -8254,10 +8254,10 @@
         <v>7.9014892798533021E-2</v>
       </c>
       <c r="O75" s="20">
-        <v>303.49936407279699</v>
+        <v>300.52724807437698</v>
       </c>
       <c r="P75" s="20">
-        <v>187.28270315242401</v>
+        <v>187.48204306283401</v>
       </c>
       <c r="Q75" s="20">
         <v>212.61599061826601</v>
@@ -8321,10 +8321,10 @@
         <v>8.1385050777985968E-2</v>
       </c>
       <c r="O76" s="20">
-        <v>311.46888740947401</v>
+        <v>316.42084151243199</v>
       </c>
       <c r="P76" s="20">
-        <v>199.283476193089</v>
+        <v>194.86386050336299</v>
       </c>
       <c r="Q76" s="20">
         <v>258.28028973982703</v>
@@ -8388,10 +8388,10 @@
         <v>9.0607862822576046E-2</v>
       </c>
       <c r="O77" s="20">
-        <v>325.92641558865301</v>
+        <v>319.59648453277902</v>
       </c>
       <c r="P77" s="20">
-        <v>209.28477991704801</v>
+        <v>206.793806141999</v>
       </c>
       <c r="Q77" s="20">
         <v>300.208260424625</v>
@@ -8455,10 +8455,10 @@
         <v>6.0592632377024003E-2</v>
       </c>
       <c r="O78" s="20">
-        <v>392.21582402850902</v>
+        <v>392.60126631356798</v>
       </c>
       <c r="P78" s="20">
-        <v>268.74617249163401</v>
+        <v>271.30687148171501</v>
       </c>
       <c r="Q78" s="20">
         <v>139.803061406296</v>
@@ -8522,10 +8522,10 @@
         <v>9.5242315048938986E-2</v>
       </c>
       <c r="O79" s="20">
-        <v>324.78542797232598</v>
+        <v>321.42763712481701</v>
       </c>
       <c r="P79" s="20">
-        <v>205.13036172306099</v>
+        <v>205.01500368398001</v>
       </c>
       <c r="Q79" s="20">
         <v>220.91147049321199</v>
@@ -8589,10 +8589,10 @@
         <v>8.6394550656399949E-2</v>
       </c>
       <c r="O80" s="20">
-        <v>341.59231997339498</v>
+        <v>335.44386278192701</v>
       </c>
       <c r="P80" s="20">
-        <v>219.846908626539</v>
+        <v>221.78200313890801</v>
       </c>
       <c r="Q80" s="20">
         <v>196.27695717063901</v>
@@ -8656,10 +8656,10 @@
         <v>8.0388982042705004E-2</v>
       </c>
       <c r="O81" s="20">
-        <v>364.98316088666098</v>
+        <v>366.67562342650803</v>
       </c>
       <c r="P81" s="20">
-        <v>246.60568560322</v>
+        <v>248.74785393781499</v>
       </c>
       <c r="Q81" s="20">
         <v>202.02297924212701</v>
@@ -8723,10 +8723,10 @@
         <v>7.5292878666116003E-2</v>
       </c>
       <c r="O82" s="20">
-        <v>503.82228481044802</v>
+        <v>502.122038282684</v>
       </c>
       <c r="P82" s="20">
-        <v>385.03982691209399</v>
+        <v>387.85153119244899</v>
       </c>
       <c r="Q82" s="20">
         <v>217.07162576877101</v>
@@ -8790,10 +8790,10 @@
         <v>6.8670034610208985E-2</v>
       </c>
       <c r="O83" s="20">
-        <v>432.69359432259398</v>
+        <v>428.83056472571798</v>
       </c>
       <c r="P83" s="20">
-        <v>300.11618191407501</v>
+        <v>298.08106131103898</v>
       </c>
       <c r="Q83" s="20">
         <v>210.927141255039</v>
@@ -8857,10 +8857,10 @@
         <v>6.6215999705074025E-2</v>
       </c>
       <c r="O84" s="20">
-        <v>351.44344910011802</v>
+        <v>357.32990906991802</v>
       </c>
       <c r="P84" s="20">
-        <v>229.22694809683099</v>
+        <v>232.67963319167501</v>
       </c>
       <c r="Q84" s="20">
         <v>161.43475014945801</v>
@@ -8924,10 +8924,10 @@
         <v>7.134131625117901E-2</v>
       </c>
       <c r="O85" s="20">
-        <v>301.43135408504401</v>
+        <v>301.96516312174498</v>
       </c>
       <c r="P85" s="20">
-        <v>194.45821498037401</v>
+        <v>188.88732623105099</v>
       </c>
       <c r="Q85" s="20">
         <v>179.24957730175799</v>
@@ -8991,10 +8991,10 @@
         <v>7.7079818497045038E-2</v>
       </c>
       <c r="O86" s="20">
-        <v>346.98869302837898</v>
+        <v>346.78133058276802</v>
       </c>
       <c r="P86" s="20">
-        <v>227.559940547845</v>
+        <v>225.18799345564199</v>
       </c>
       <c r="Q86" s="20">
         <v>226.757094670367</v>
@@ -9058,10 +9058,10 @@
         <v>6.838793777671498E-2</v>
       </c>
       <c r="O87" s="20">
-        <v>361.74167894332999</v>
+        <v>361.64212548588102</v>
       </c>
       <c r="P87" s="20">
-        <v>244.98669965279899</v>
+        <v>240.201375551437</v>
       </c>
       <c r="Q87" s="20">
         <v>200.07181859034301</v>
@@ -9125,10 +9125,10 @@
         <v>6.383979596454098E-2</v>
       </c>
       <c r="O88" s="20">
-        <v>408.182099157793</v>
+        <v>409.27016593354699</v>
       </c>
       <c r="P88" s="20">
-        <v>284.37885374949298</v>
+        <v>288.00046908184601</v>
       </c>
       <c r="Q88" s="20">
         <v>176.462279139527</v>
@@ -9192,10 +9192,10 @@
         <v>6.1848278493864983E-2</v>
       </c>
       <c r="O89" s="20">
-        <v>507.28734030317003</v>
+        <v>501.36478054983201</v>
       </c>
       <c r="P89" s="20">
-        <v>377.78907876024999</v>
+        <v>382.69328550326497</v>
       </c>
       <c r="Q89" s="20">
         <v>222.879033981432</v>
@@ -9259,10 +9259,10 @@
         <v>8.0649306840874013E-2</v>
       </c>
       <c r="O90" s="20">
-        <v>379.91112348980801</v>
+        <v>383.31534161451299</v>
       </c>
       <c r="P90" s="20">
-        <v>258.35195322883499</v>
+        <v>260.29421138067403</v>
       </c>
       <c r="Q90" s="20">
         <v>189.23349551051999</v>
@@ -9326,10 +9326,10 @@
         <v>7.8088475407524949E-2</v>
       </c>
       <c r="O91" s="20">
-        <v>354.42736404199201</v>
+        <v>361.29136698987099</v>
       </c>
       <c r="P91" s="20">
-        <v>240.45651192800801</v>
+        <v>239.92943290522101</v>
       </c>
       <c r="Q91" s="20">
         <v>191.45132804269201</v>
@@ -9393,10 +9393,10 @@
         <v>6.8879796660878956E-2</v>
       </c>
       <c r="O92" s="20">
-        <v>381.51493702989802</v>
+        <v>377.45162287386898</v>
       </c>
       <c r="P92" s="20">
-        <v>261.76993921503799</v>
+        <v>258.89585038995102</v>
       </c>
       <c r="Q92" s="20">
         <v>190.87777177846701</v>
@@ -9460,10 +9460,10 @@
         <v>6.3234936243403039E-2</v>
       </c>
       <c r="O93" s="20">
-        <v>363.995055691397</v>
+        <v>359.16276144944601</v>
       </c>
       <c r="P93" s="20">
-        <v>244.17569439424901</v>
+        <v>247.36189864117</v>
       </c>
       <c r="Q93" s="20">
         <v>147.69771691236701</v>
@@ -9527,10 +9527,10 @@
         <v>6.5799125469704012E-2</v>
       </c>
       <c r="O94" s="20">
-        <v>311.71856113300203</v>
+        <v>311.99241593924501</v>
       </c>
       <c r="P94" s="20">
-        <v>198.36752771026801</v>
+        <v>196.72967150161699</v>
       </c>
       <c r="Q94" s="20">
         <v>177.85120011768899</v>
@@ -9594,10 +9594,10 @@
         <v>6.8115063385765007E-2</v>
       </c>
       <c r="O95" s="20">
-        <v>336.190055588581</v>
+        <v>330.85339684648397</v>
       </c>
       <c r="P95" s="20">
-        <v>217.12522876542999</v>
+        <v>214.70646680761399</v>
       </c>
       <c r="Q95" s="20">
         <v>154.86548474292201</v>
@@ -9661,10 +9661,10 @@
         <v>0.10998797455572495</v>
       </c>
       <c r="O96" s="20">
-        <v>323.10276466264901</v>
+        <v>324.219356817164</v>
       </c>
       <c r="P96" s="20">
-        <v>210.381139565121</v>
+        <v>210.89567889065299</v>
       </c>
       <c r="Q96" s="20">
         <v>254.36241017216901</v>
@@ -9728,10 +9728,10 @@
         <v>0.10259454704138005</v>
       </c>
       <c r="O97" s="20">
-        <v>322.06109356596102</v>
+        <v>324.20355910024398</v>
       </c>
       <c r="P97" s="20">
-        <v>206.28290160304499</v>
+        <v>205.97528854470201</v>
       </c>
       <c r="Q97" s="20">
         <v>256.826241277534</v>
@@ -9795,10 +9795,10 @@
         <v>6.6366232051452978E-2</v>
       </c>
       <c r="O98" s="20">
-        <v>362.51774988255102</v>
+        <v>360.53744952678102</v>
       </c>
       <c r="P98" s="20">
-        <v>240.86872930451199</v>
+        <v>241.410659876214</v>
       </c>
       <c r="Q98" s="20">
         <v>176.366966707084</v>
@@ -9862,10 +9862,10 @@
         <v>7.0486902789034078E-2</v>
       </c>
       <c r="O99" s="20">
-        <v>358.87975137223901</v>
+        <v>361.17078646405201</v>
       </c>
       <c r="P99" s="20">
-        <v>237.07572806062001</v>
+        <v>235.213177046006</v>
       </c>
       <c r="Q99" s="20">
         <v>197.33258560190001</v>
@@ -9929,10 +9929,10 @@
         <v>7.6541794033265997E-2</v>
       </c>
       <c r="O100" s="20">
-        <v>282.801526487839</v>
+        <v>285.24339402855401</v>
       </c>
       <c r="P100" s="20">
-        <v>172.12670087527101</v>
+        <v>176.223538787482</v>
       </c>
       <c r="Q100" s="20">
         <v>207.076153845916</v>
@@ -9996,10 +9996,10 @@
         <v>6.1898149802629088E-2</v>
       </c>
       <c r="O101" s="20">
-        <v>405.83413520590602</v>
+        <v>403.79387468342497</v>
       </c>
       <c r="P101" s="20">
-        <v>280.20548300627098</v>
+        <v>278.648048511387</v>
       </c>
       <c r="Q101" s="20">
         <v>242.76415209097999</v>
@@ -10063,10 +10063,10 @@
         <v>6.4862008491037015E-2</v>
       </c>
       <c r="O102" s="20">
-        <v>389.56954283728902</v>
+        <v>386.76580300749998</v>
       </c>
       <c r="P102" s="20">
-        <v>268.48285648526502</v>
+        <v>268.02409546039001</v>
       </c>
       <c r="Q102" s="20">
         <v>167.46710890599201</v>
@@ -10130,10 +10130,10 @@
         <v>7.1923197595546995E-2</v>
       </c>
       <c r="O103" s="20">
-        <v>362.96121909720199</v>
+        <v>357.21581090913901</v>
       </c>
       <c r="P103" s="20">
-        <v>235.05592958682001</v>
+        <v>238.32037751289499</v>
       </c>
       <c r="Q103" s="20">
         <v>234.909434966124</v>
@@ -10197,10 +10197,10 @@
         <v>7.5498747196985017E-2</v>
       </c>
       <c r="O104" s="20">
-        <v>323.47840949865798</v>
+        <v>326.54266132225598</v>
       </c>
       <c r="P104" s="20">
-        <v>207.08063282117999</v>
+        <v>205.113500312231</v>
       </c>
       <c r="Q104" s="20">
         <v>209.15153906871501</v>
@@ -10264,10 +10264,10 @@
         <v>6.6080019748803009E-2</v>
       </c>
       <c r="O105" s="20">
-        <v>422.88712215871698</v>
+        <v>426.15348127255402</v>
       </c>
       <c r="P105" s="20">
-        <v>303.08505687060199</v>
+        <v>301.493038254591</v>
       </c>
       <c r="Q105" s="20">
         <v>235.14208562472001</v>
@@ -10331,10 +10331,10 @@
         <v>6.7666287637870082E-2</v>
       </c>
       <c r="O106" s="20">
-        <v>383.84489059180902</v>
+        <v>383.83566895147101</v>
       </c>
       <c r="P106" s="20">
-        <v>262.49686960658499</v>
+        <v>263.48858965212202</v>
       </c>
       <c r="Q106" s="20">
         <v>227.70616625545699</v>
@@ -10398,10 +10398,10 @@
         <v>6.921505700901498E-2</v>
       </c>
       <c r="O107" s="20">
-        <v>353.83417444769299</v>
+        <v>357.09651534854203</v>
       </c>
       <c r="P107" s="20">
-        <v>238.08408871316701</v>
+        <v>239.382905957627</v>
       </c>
       <c r="Q107" s="20">
         <v>203.605788789212</v>
@@ -10465,10 +10465,10 @@
         <v>7.1618143766958964E-2</v>
       </c>
       <c r="O108" s="20">
-        <v>393.1077213625</v>
+        <v>388.34563608569903</v>
       </c>
       <c r="P108" s="20">
-        <v>270.58287978586901</v>
+        <v>276.17787763839499</v>
       </c>
       <c r="Q108" s="20">
         <v>237.54599099214201</v>
@@ -10532,10 +10532,10 @@
         <v>7.4421488641383982E-2</v>
       </c>
       <c r="O109" s="20">
-        <v>341.56370891699902</v>
+        <v>339.15825202157799</v>
       </c>
       <c r="P109" s="20">
-        <v>218.58223483050901</v>
+        <v>225.375715447998</v>
       </c>
       <c r="Q109" s="20">
         <v>218.64850007768399</v>
@@ -10599,10 +10599,10 @@
         <v>7.1999699496857028E-2</v>
       </c>
       <c r="O110" s="20">
-        <v>317.224778306205</v>
+        <v>316.12844862941699</v>
       </c>
       <c r="P110" s="20">
-        <v>200.16587371131101</v>
+        <v>199.93574561945101</v>
       </c>
       <c r="Q110" s="20">
         <v>215.46714905689299</v>
@@ -10666,10 +10666,10 @@
         <v>9.1818943703867006E-2</v>
       </c>
       <c r="O111" s="20">
-        <v>354.12452807037801</v>
+        <v>348.18561471987402</v>
       </c>
       <c r="P111" s="20">
-        <v>231.382767932158</v>
+        <v>236.104770821567</v>
       </c>
       <c r="Q111" s="20">
         <v>241.319950846952</v>
@@ -10733,10 +10733,10 @@
         <v>8.9503560141881988E-2</v>
       </c>
       <c r="O112" s="20">
-        <v>317.22643113453199</v>
+        <v>316.72400562604201</v>
       </c>
       <c r="P112" s="20">
-        <v>204.11400172477599</v>
+        <v>200.68382408102801</v>
       </c>
       <c r="Q112" s="20">
         <v>276.209143671611</v>
@@ -10800,10 +10800,10 @@
         <v>7.6501282086354983E-2</v>
       </c>
       <c r="O113" s="20">
-        <v>341.76635791548199</v>
+        <v>346.383681580158</v>
       </c>
       <c r="P113" s="20">
-        <v>229.67658765005001</v>
+        <v>226.200020957546</v>
       </c>
       <c r="Q113" s="20">
         <v>213.34534984011</v>
@@ -10867,10 +10867,10 @@
         <v>6.8836326873821019E-2</v>
       </c>
       <c r="O114" s="20">
-        <v>403.530090801254</v>
+        <v>405.63648770136803</v>
       </c>
       <c r="P114" s="20">
-        <v>276.37644363647701</v>
+        <v>281.202276761966</v>
       </c>
       <c r="Q114" s="20">
         <v>259.82092945658798</v>
@@ -10934,10 +10934,10 @@
         <v>7.6002567674056998E-2</v>
       </c>
       <c r="O115" s="20">
-        <v>344.48085304562699</v>
+        <v>343.066826469153</v>
       </c>
       <c r="P115" s="20">
-        <v>224.030073652076</v>
+        <v>225.47647528232699</v>
       </c>
       <c r="Q115" s="20">
         <v>241.58208909061901</v>
@@ -11001,10 +11001,10 @@
         <v>7.4910041444648967E-2</v>
       </c>
       <c r="O116" s="20">
-        <v>347.644483667945</v>
+        <v>344.40015983677102</v>
       </c>
       <c r="P116" s="20">
-        <v>230.92631229958801</v>
+        <v>234.89567387485499</v>
       </c>
       <c r="Q116" s="20">
         <v>214.616179026179</v>
@@ -11068,10 +11068,10 @@
         <v>6.207405961357898E-2</v>
       </c>
       <c r="O117" s="20">
-        <v>426.93627970082298</v>
+        <v>432.23467836114901</v>
       </c>
       <c r="P117" s="20">
-        <v>303.90436878257401</v>
+        <v>300.731947807886</v>
       </c>
       <c r="Q117" s="20">
         <v>229.48912834067301</v>
@@ -11135,10 +11135,10 @@
         <v>6.6495210156468976E-2</v>
       </c>
       <c r="O118" s="20">
-        <v>366.926595125711</v>
+        <v>371.99895669187299</v>
       </c>
       <c r="P118" s="20">
-        <v>243.21333485533901</v>
+        <v>251.69597102424299</v>
       </c>
       <c r="Q118" s="20">
         <v>204.79562217798801</v>
@@ -11202,10 +11202,10 @@
         <v>7.0883400179238998E-2</v>
       </c>
       <c r="O119" s="20">
-        <v>356.76223884360599</v>
+        <v>362.76311574852599</v>
       </c>
       <c r="P119" s="20">
-        <v>236.51961328742701</v>
+        <v>233.75902942803299</v>
       </c>
       <c r="Q119" s="20">
         <v>213.04464747397</v>
@@ -11269,10 +11269,10 @@
         <v>7.0310658619782918E-2</v>
       </c>
       <c r="O120" s="20">
-        <v>343.53286308433098</v>
+        <v>342.85203574519602</v>
       </c>
       <c r="P120" s="20">
-        <v>223.55043942503099</v>
+        <v>219.92967170344701</v>
       </c>
       <c r="Q120" s="20">
         <v>235.654654908282</v>
@@ -11336,10 +11336,10 @@
         <v>8.2261990793522033E-2</v>
       </c>
       <c r="O121" s="20">
-        <v>306.93486883064497</v>
+        <v>304.64233408801101</v>
       </c>
       <c r="P121" s="20">
-        <v>191.829431593827</v>
+        <v>191.46630059265999</v>
       </c>
       <c r="Q121" s="20">
         <v>227.39899140982601</v>
@@ -11403,10 +11403,10 @@
         <v>7.5823235631216956E-2</v>
       </c>
       <c r="O122" s="20">
-        <v>345.04601300896502</v>
+        <v>342.34650442338199</v>
       </c>
       <c r="P122" s="20">
-        <v>227.730174568363</v>
+        <v>223.766043197887</v>
       </c>
       <c r="Q122" s="20">
         <v>258.28368495362599</v>
@@ -11470,10 +11470,10 @@
         <v>8.4296101049905037E-2</v>
       </c>
       <c r="O123" s="20">
-        <v>352.81121523424298</v>
+        <v>362.05104097237302</v>
       </c>
       <c r="P123" s="20">
-        <v>229.878286702157</v>
+        <v>236.56882347406199</v>
       </c>
       <c r="Q123" s="20">
         <v>283.18054731770798</v>
@@ -11537,10 +11537,10 @@
         <v>7.4730726478686949E-2</v>
       </c>
       <c r="O124" s="20">
-        <v>320.313990459031</v>
+        <v>320.862171065631</v>
       </c>
       <c r="P124" s="20">
-        <v>205.891958650959</v>
+        <v>205.04540804555501</v>
       </c>
       <c r="Q124" s="20">
         <v>177.227077130563</v>
@@ -11604,10 +11604,10 @@
         <v>7.2928282084535001E-2</v>
       </c>
       <c r="O125" s="20">
-        <v>338.62922501016101</v>
+        <v>339.798253975629</v>
       </c>
       <c r="P125" s="20">
-        <v>218.845847150336</v>
+        <v>224.59233370657901</v>
       </c>
       <c r="Q125" s="20">
         <v>182.96470675222801</v>
@@ -11671,10 +11671,10 @@
         <v>5.7340986581808029E-2</v>
       </c>
       <c r="O126" s="20">
-        <v>377.336077715469</v>
+        <v>374.94965576079602</v>
       </c>
       <c r="P126" s="20">
-        <v>255.57063738709601</v>
+        <v>255.758644012736</v>
       </c>
       <c r="Q126" s="20">
         <v>184.74293929316201</v>
@@ -11738,10 +11738,10 @@
         <v>7.1976750514567978E-2</v>
       </c>
       <c r="O127" s="20">
-        <v>348.85277758039501</v>
+        <v>350.19782698393101</v>
       </c>
       <c r="P127" s="20">
-        <v>228.04314582240801</v>
+        <v>232.04497715270901</v>
       </c>
       <c r="Q127" s="20">
         <v>223.45675842361101</v>
@@ -11805,10 +11805,10 @@
         <v>6.4840353290535058E-2</v>
       </c>
       <c r="O128" s="20">
-        <v>331.80975049909802</v>
+        <v>331.40705743128399</v>
       </c>
       <c r="P128" s="20">
-        <v>217.854309042967</v>
+        <v>220.49280407392899</v>
       </c>
       <c r="Q128" s="20">
         <v>189.34532409826599</v>
@@ -11872,10 +11872,10 @@
         <v>6.6519038205504089E-2</v>
       </c>
       <c r="O129" s="20">
-        <v>389.028345282651</v>
+        <v>392.75339396762001</v>
       </c>
       <c r="P129" s="20">
-        <v>270.33440344235697</v>
+        <v>266.74295381368802</v>
       </c>
       <c r="Q129" s="20">
         <v>250.50254164172901</v>
@@ -11939,10 +11939,10 @@
         <v>8.8194591726218019E-2</v>
       </c>
       <c r="O130" s="20">
-        <v>309.58472583754002</v>
+        <v>303.78033353550597</v>
       </c>
       <c r="P130" s="20">
-        <v>192.90524742337399</v>
+        <v>191.452749980855</v>
       </c>
       <c r="Q130" s="20">
         <v>307.04327749924101</v>
@@ -12006,10 +12006,10 @@
         <v>8.2900221654080064E-2</v>
       </c>
       <c r="O131" s="20">
-        <v>301.38039579195998</v>
+        <v>298.40913228105501</v>
       </c>
       <c r="P131" s="20">
-        <v>184.70895743238199</v>
+        <v>183.57695297580199</v>
       </c>
       <c r="Q131" s="20">
         <v>255.17505369783601</v>
@@ -12073,10 +12073,10 @@
         <v>6.9523188877936959E-2</v>
       </c>
       <c r="O132" s="20">
-        <v>355.93940335159698</v>
+        <v>349.72791340720602</v>
       </c>
       <c r="P132" s="20">
-        <v>238.205561808162</v>
+        <v>237.23263370995301</v>
       </c>
       <c r="Q132" s="20">
         <v>246.38916519918101</v>
@@ -12140,10 +12140,10 @@
         <v>8.2210411538369943E-2</v>
       </c>
       <c r="O133" s="20">
-        <v>293.51022399700099</v>
+        <v>293.548530279754</v>
       </c>
       <c r="P133" s="20">
-        <v>178.36449554923999</v>
+        <v>183.064018725664</v>
       </c>
       <c r="Q133" s="20">
         <v>226.196024867055</v>
@@ -12207,10 +12207,10 @@
         <v>8.0804441057626963E-2</v>
       </c>
       <c r="O134" s="20">
-        <v>349.31464906542902</v>
+        <v>342.94958094547798</v>
       </c>
       <c r="P134" s="20">
-        <v>235.368048732745</v>
+        <v>225.53485511701999</v>
       </c>
       <c r="Q134" s="20">
         <v>263.32441187036102</v>
@@ -12274,10 +12274,10 @@
         <v>8.0154191112080109E-2</v>
       </c>
       <c r="O135" s="20">
-        <v>282.473940300663</v>
+        <v>282.48908427619199</v>
       </c>
       <c r="P135" s="20">
-        <v>170.90031249876699</v>
+        <v>173.55582204195699</v>
       </c>
       <c r="Q135" s="20">
         <v>232.660430580222</v>
@@ -12341,10 +12341,10 @@
         <v>8.193312105707895E-2</v>
       </c>
       <c r="O136" s="20">
-        <v>337.66453214445602</v>
+        <v>331.66941529649699</v>
       </c>
       <c r="P136" s="20">
-        <v>218.04670017770701</v>
+        <v>219.68866390431799</v>
       </c>
       <c r="Q136" s="20">
         <v>317.443831574721</v>
@@ -12408,10 +12408,10 @@
         <v>7.3432914924053017E-2</v>
       </c>
       <c r="O137" s="20">
-        <v>348.85720368481799</v>
+        <v>345.39314578305999</v>
       </c>
       <c r="P137" s="20">
-        <v>226.02153335333401</v>
+        <v>223.86459156111599</v>
       </c>
       <c r="Q137" s="20">
         <v>248.912186569244</v>
@@ -12475,10 +12475,10 @@
         <v>6.8326663311566005E-2</v>
       </c>
       <c r="O138" s="20">
-        <v>397.40914874455802</v>
+        <v>398.85373011837299</v>
       </c>
       <c r="P138" s="20">
-        <v>273.84055652487098</v>
+        <v>276.05094385704302</v>
       </c>
       <c r="Q138" s="20">
         <v>231.16784807084699</v>
@@ -12542,10 +12542,10 @@
         <v>0.10251090173706401</v>
       </c>
       <c r="O139" s="20">
-        <v>329.80436974692901</v>
+        <v>327.60375656216598</v>
       </c>
       <c r="P139" s="20">
-        <v>215.769095339427</v>
+        <v>210.60042881150201</v>
       </c>
       <c r="Q139" s="20">
         <v>340.445448543792</v>
@@ -12609,10 +12609,10 @@
         <v>9.1666520743985069E-2</v>
       </c>
       <c r="O140" s="20">
-        <v>333.131774101117</v>
+        <v>332.73763999163998</v>
       </c>
       <c r="P140" s="20">
-        <v>214.00054074179599</v>
+        <v>214.251679224062</v>
       </c>
       <c r="Q140" s="20">
         <v>260.650686583327</v>
@@ -12676,10 +12676,10 @@
         <v>7.1180829122023059E-2</v>
       </c>
       <c r="O141" s="20">
-        <v>408.20693158814601</v>
+        <v>416.30870532884501</v>
       </c>
       <c r="P141" s="20">
-        <v>289.44467169021698</v>
+        <v>288.23527436749998</v>
       </c>
       <c r="Q141" s="20">
         <v>299.88384552799403</v>
@@ -12743,10 +12743,10 @@
         <v>7.4013504216770998E-2</v>
       </c>
       <c r="O142" s="20">
-        <v>340.96979590729501</v>
+        <v>339.45592154412799</v>
       </c>
       <c r="P142" s="20">
-        <v>222.42699727096701</v>
+        <v>220.27709329858499</v>
       </c>
       <c r="Q142" s="20">
         <v>269.45565822468598</v>

</xml_diff>